<commit_message>
Update insert_normunit for commercial building type compatibility.
</commit_message>
<xml_diff>
--- a/scripts/data transformation/NumStor2.xlsx
+++ b/scripts/data transformation/NumStor2.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nfette\Desktop\Training20230815\deer-dev-post-process\scripts\data transformation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEER2026\SWHC001-05-submission1\scripts\data transformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3F7ED025-C09F-4445-B09A-7A9C038A5A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A55A390-3BA0-4DCD-B718-0DD9BC36431B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31680" yWindow="1275" windowWidth="21600" windowHeight="13125"/>
+    <workbookView xWindow="11880" yWindow="315" windowWidth="16845" windowHeight="14730" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NumStor" sheetId="1" r:id="rId1"/>
+    <sheet name="NumBldgs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="56">
   <si>
     <t>BldgType</t>
   </si>
@@ -104,12 +118,96 @@
   </si>
   <si>
     <t>MFm</t>
+  </si>
+  <si>
+    <t>numbldgs</t>
+  </si>
+  <si>
+    <t>Dmo</t>
+  </si>
+  <si>
+    <t>Asm</t>
+  </si>
+  <si>
+    <t>ECC</t>
+  </si>
+  <si>
+    <t>EPr</t>
+  </si>
+  <si>
+    <t>ERC</t>
+  </si>
+  <si>
+    <t>ESe</t>
+  </si>
+  <si>
+    <t>EUn</t>
+  </si>
+  <si>
+    <t>Hsp</t>
+  </si>
+  <si>
+    <t>Htl</t>
+  </si>
+  <si>
+    <t>MBT</t>
+  </si>
+  <si>
+    <t>MLI</t>
+  </si>
+  <si>
+    <t>Mtl</t>
+  </si>
+  <si>
+    <t>Nrs</t>
+  </si>
+  <si>
+    <t>OfL</t>
+  </si>
+  <si>
+    <t>OfS</t>
+  </si>
+  <si>
+    <t>RFF</t>
+  </si>
+  <si>
+    <t>RSD</t>
+  </si>
+  <si>
+    <t>Rt3</t>
+  </si>
+  <si>
+    <t>RtL</t>
+  </si>
+  <si>
+    <t>RtS</t>
+  </si>
+  <si>
+    <t>SCn</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t>Gro</t>
+  </si>
+  <si>
+    <t>Lib</t>
+  </si>
+  <si>
+    <t>Rel</t>
+  </si>
+  <si>
+    <t>SUn</t>
+  </si>
+  <si>
+    <t>WRf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -648,9 +746,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -688,7 +786,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -794,7 +892,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -936,17 +1034,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="N114" sqref="N114"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1790,7 +1890,7 @@
         <v>1.48</v>
       </c>
       <c r="G35">
-        <f t="shared" ref="G35:G97" si="1">(B35=2)*(F35-1)+(B35=1)*(2-F35)</f>
+        <f t="shared" ref="G35:G65" si="1">(B35=2)*(F35-1)+(B35=1)*(2-F35)</f>
         <v>0.48</v>
       </c>
     </row>
@@ -3791,6 +3891,261 @@
         <v>1</v>
       </c>
       <c r="G129">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C193CD-3CA4-461A-A98B-E380473B1343}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B5:B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30">
         <v>1</v>
       </c>
     </row>

</xml_diff>